<commit_message>
Modified the logic for handling items by order
Modified the logic for handling items by order
</commit_message>
<xml_diff>
--- a/Yahoo/src/test/resources/Automation TestData.xlsx
+++ b/Yahoo/src/test/resources/Automation TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shama\Documents\GitHub\DBiz\DBiz-Assessment_Latest\Yahoo\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E560796-2E1A-4CB1-8184-11F3221F6360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9970C3-FC28-48BD-9BA5-6949FC4FD36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>StockFullName</t>
+  </si>
+  <si>
+    <t>PriceExceedBy</t>
   </si>
 </sst>
 </file>
@@ -372,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -384,9 +387,10 @@
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -399,8 +403,11 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -412,6 +419,9 @@
       </c>
       <c r="D2">
         <v>1</v>
+      </c>
+      <c r="E2">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>